<commit_message>
[imp] update style of btn GPS-23
</commit_message>
<xml_diff>
--- a/assets/files/products2024.03.18.xlsx
+++ b/assets/files/products2024.03.18.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sovannarith.penh\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khav.saroeun\Desktop\team\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,15 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Pizza</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Apple</t>
-  </si>
-  <si>
-    <t>orange</t>
   </si>
 </sst>
 </file>
@@ -129,94 +123,6 @@
         <a:xfrm>
           <a:off x="4857750" y="295275"/>
           <a:ext cx="676275" cy="381000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>458304</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>107675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1176130</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>604631</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4848087" y="819979"/>
-          <a:ext cx="717826" cy="496956"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>458304</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>107675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1176130</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>604631</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5229087" y="629479"/>
-          <a:ext cx="717826" cy="496956"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -497,16 +403,16 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="13.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="18.81640625" customWidth="1"/>
-    <col min="6" max="6" width="19.26953125" customWidth="1"/>
-    <col min="7" max="7" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1">
         <v>121212</v>
@@ -515,7 +421,7 @@
         <v>3</v>
       </c>
       <c r="D1">
-        <v>37</v>
+        <v>168</v>
       </c>
       <c r="E1">
         <v>47</v>
@@ -527,51 +433,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>121212</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>37</v>
-      </c>
-      <c r="E2">
-        <v>47</v>
-      </c>
-      <c r="G2" s="1">
-        <v>45570</v>
-      </c>
-      <c r="H2">
-        <v>300</v>
-      </c>
+    <row r="2" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>121212</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>37</v>
-      </c>
-      <c r="E3">
-        <v>47</v>
-      </c>
-      <c r="G3" s="1">
-        <v>45571</v>
-      </c>
-      <c r="H3">
-        <v>301</v>
-      </c>
+    <row r="3" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>